<commit_message>
Refactoring of Framework of Lesoon 4
</commit_message>
<xml_diff>
--- a/AndyTEST/Libs/UserStoriesChecklist_02.xlsx
+++ b/AndyTEST/Libs/UserStoriesChecklist_02.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView windowHeight="8010" windowWidth="14805" xWindow="240" yWindow="105"/>
   </bookViews>
   <sheets>
-    <sheet name="Story 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Story 2" sheetId="2" r:id="rId2"/>
-    <sheet name="Story 3" sheetId="3" r:id="rId3"/>
+    <sheet name="Story 1" r:id="rId1" sheetId="1"/>
+    <sheet name="Story 2" r:id="rId2" sheetId="2"/>
+    <sheet name="Story 3" r:id="rId3" sheetId="3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="54">
   <si>
     <t>Test Case №</t>
   </si>
@@ -45,9 +45,6 @@
     <t>4.</t>
   </si>
   <si>
-    <t>SELECT flightNumber FROM Flights WHERE departureAirport = 'London' AND arrivalAirport = 'Munich';</t>
-  </si>
-  <si>
     <t>5.</t>
   </si>
   <si>
@@ -60,36 +57,24 @@
     <t>Check the priority boarding for flight from London airport.</t>
   </si>
   <si>
-    <t>SELECT priorityBoarding FROM Airports WHERE airport = 'London';</t>
-  </si>
-  <si>
     <t>yes;</t>
   </si>
   <si>
     <t>Check the average ticket price for flight from London to Munich less than 120 Euro.</t>
   </si>
   <si>
-    <t>SELECT averageTicketPrice FROM Flights WHERE departureAirport = 'London' AND arrivalAirport = 'Munich' AND averageTicketPrice &lt; 120;</t>
-  </si>
-  <si>
     <t>90;</t>
   </si>
   <si>
     <t>Check the available seats for flight from London to Munich more than 3.</t>
   </si>
   <si>
-    <t>SELECT availableSeats FROM Flights WHERE availableSeats &gt; 3 AND departureAirport = 'London' AND arrivalAirport = 'Munich';</t>
-  </si>
-  <si>
     <t>12;</t>
   </si>
   <si>
     <t>Check the additional space service for flight from London to Munich.</t>
   </si>
   <si>
-    <t>SELECT Flights.flightNumber, additionalSpaceService FROM Flights INNER JOIN Airlines ON Flights.flightNumber = Airlines.flightnumber WHERE departureAirport  = 'London' AND arrivalAirport  = 'Munich'</t>
-  </si>
-  <si>
     <t>1001;yes;</t>
   </si>
   <si>
@@ -102,66 +87,42 @@
     <t>Check the flight number with departure from New York.</t>
   </si>
   <si>
-    <t>SELECT flightNumber FROM Flights WHERE departureAirport = 'New York'</t>
-  </si>
-  <si>
     <t>1005;1006;1007;1008;1009;1010;</t>
   </si>
   <si>
     <t>Check the flight number without stops from New York.</t>
   </si>
   <si>
-    <t>SELECT flightNumber FROM Flights WHERE departureAirport = 'New York' AND stopsNumber = 0</t>
-  </si>
-  <si>
     <t>1008;</t>
   </si>
   <si>
     <t>Check the flight less than 500 Euro from New York.</t>
   </si>
   <si>
-    <t>SELECT flightNumber FROM Flights WHERE averageTicketPrice &lt; 500 AND departureAirport = 'New York'</t>
-  </si>
-  <si>
     <t>1006;1007;1008;1009;1010;</t>
   </si>
   <si>
     <t>Check the flight with in-flight food service from New York.</t>
   </si>
   <si>
-    <t>SELECT Flights.flightNumber FROM Flights INNER JOIN Airlines ON Flights.flightNumber = Airlines.flightNumber WHERE departureAirport = 'New York' AND isMealincluded = 'yes'</t>
-  </si>
-  <si>
     <t>1005;1006;1007;1008;1010;</t>
   </si>
   <si>
     <t>Check the flights from New York and where the Duty Free shops are in the destination airport.</t>
   </si>
   <si>
-    <t>SELECT flightNumber, arrivalAirport FROM Flights INNER JOIN Airports ON Flights.airportNumber = Airports.airportNumber WHERE  dutyFree = 'yes'</t>
-  </si>
-  <si>
     <t>1006;1007;1008;1009;</t>
   </si>
   <si>
     <t>Check the airlines which provide flight to Milan and Helsinki.</t>
   </si>
   <si>
-    <t>SELECT airline FROM Airlines INNER JOIN Flights ON Airlines.flightNumber = Flights.flightNumber WHERE arrivalAirport IN('Milan', 'Helsinki') GROUP BY airline</t>
-  </si>
-  <si>
     <t>Check the airlines with web registration of boarding pass which provide flight to Milan and Helsinki.</t>
   </si>
   <si>
-    <t>SELECT airline FROM Airlines INNER JOIN Flights ON Airlines.flightNumber = Flights.flightNumber WHERE arrivalAirport IN ('Milan' , 'Helsinki' ) AND webRegistration = 'yes' GROUP BY airline</t>
-  </si>
-  <si>
     <t>Check the airlines with average tickets price of less than 100 Euro.</t>
   </si>
   <si>
-    <t>SELECT airline FROM Airlines INNER JOIN Flights ON Airlines.flightNumber = Flights.flightNumber GROUP BY airline HAVING AVG(averageTicketPrice) &lt; 100</t>
-  </si>
-  <si>
     <t>Air France;AirAsia;Cathay Pacific;Emirates;Lufthansa;Virgin;Windrose Aero;</t>
   </si>
   <si>
@@ -169,13 +130,62 @@
   </si>
   <si>
     <t>Turkish Airlines;</t>
+  </si>
+  <si>
+    <t>USE TestDB SELECT flightNumber FROM Flights WHERE departureAirport = 'London' AND arrivalAirport = 'Munich';</t>
+  </si>
+  <si>
+    <t>USE TestDB SELECT priorityBoarding FROM Airports WHERE airport = 'London';</t>
+  </si>
+  <si>
+    <t>USE TestDB SELECT averageTicketPrice FROM Flights WHERE departureAirport = 'London' AND arrivalAirport = 'Munich' AND averageTicketPrice &lt; 120;</t>
+  </si>
+  <si>
+    <t>USE TestDB SELECT availableSeats FROM Flights WHERE availableSeats &gt; 3 AND departureAirport = 'London' AND arrivalAirport = 'Munich';</t>
+  </si>
+  <si>
+    <t>USE TestDB SELECT Flights.flightNumber, additionalSpaceService FROM Flights INNER JOIN Airlines ON Flights.flightNumber = Airlines.flightnumber WHERE departureAirport  = 'London' AND arrivalAirport  = 'Munich'</t>
+  </si>
+  <si>
+    <t>USE TestDB SELECT flightNumber FROM Flights WHERE departureAirport = 'New York'</t>
+  </si>
+  <si>
+    <t>USE TestDB SELECT flightNumber FROM Flights WHERE departureAirport = 'New York' AND stopsNumber = 0</t>
+  </si>
+  <si>
+    <t>USE TestDB SELECT flightNumber FROM Flights WHERE averageTicketPrice &lt; 500 AND departureAirport = 'New York'</t>
+  </si>
+  <si>
+    <t>USE TestDB SELECT Flights.flightNumber FROM Flights INNER JOIN Airlines ON Flights.flightNumber = Airlines.flightNumber WHERE departureAirport = 'New York' AND isMealincluded = 'yes'</t>
+  </si>
+  <si>
+    <t>USE TestDB SELECT flightNumber, arrivalAirport FROM Flights INNER JOIN Airports ON Flights.airportNumber = Airports.airportNumber WHERE  dutyFree = 'yes'</t>
+  </si>
+  <si>
+    <t>USE TestDB SELECT airline FROM Airlines INNER JOIN Flights ON Airlines.flightNumber = Flights.flightNumber WHERE arrivalAirport IN('Milan', 'Helsinki') GROUP BY airline</t>
+  </si>
+  <si>
+    <t>USE TestDB SELECT airline FROM Airlines INNER JOIN Flights ON Airlines.flightNumber = Flights.flightNumber WHERE arrivalAirport IN ('Milan' , 'Helsinki' ) AND webRegistration = 'yes' GROUP BY airline</t>
+  </si>
+  <si>
+    <t>USE TestDB SELECT airline FROM Airlines INNER JOIN Flights ON Airlines.flightNumber = Flights.flightNumber GROUP BY airline HAVING AVG(averageTicketPrice) &lt; 100</t>
+  </si>
+  <si>
+    <t>1001;Munich;1002;New York;1003;Ottava;1004;Milan;1011;London;1012;Kiev;1013;Vilnius;1019;Ottava;1020;Vilnius;1021;Helsinki;1022;New York;1023;New York;1024;Milan;1025;London;1029;Kiev;1030;Helsinki;1031;Ottava;1033;Beijing;1034;Sydney;1035;Munich;</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,31 +224,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="17"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="17"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="17"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="17"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="17"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color indexed="10"/>
       <name val="Calibri"/>
     </font>
@@ -257,8 +242,98 @@
       <color indexed="17"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
   </fonts>
-  <fills count="22">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -303,71 +378,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FF00FF80"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FF00FF80"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FF00FF80"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FF00FF80"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FF00FF80"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FF00FF80"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FF00FF80"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FF00FF80"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FF00FF80"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="12"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FF00FF80"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FF00FF80"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FF00FF80"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -394,95 +404,108 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="49">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="1" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="3" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="4" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="5" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="6" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="7" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="8" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="23" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="24" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="26" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Обычный" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -499,10 +522,10 @@
   <a:themeElements>
     <a:clrScheme name="Стандартная">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -537,7 +560,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -572,7 +595,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -660,7 +683,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -669,13 +692,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -685,7 +708,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -694,7 +717,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -703,7 +726,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -713,12 +736,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -749,7 +772,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -768,7 +791,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -780,22 +803,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="10" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.42578125" style="10" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="36.42578125" style="10" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.42578125" style="10" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.85546875" style="10" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.140625" style="10" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9.140625" style="10" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="10" width="13.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="10" width="33.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="10" width="36.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="10" width="22.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="10" width="16.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="10" width="18.140625" collapsed="true"/>
+    <col min="7" max="16384" style="10" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -815,118 +838,138 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G1" s="9"/>
     </row>
-    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row ht="45" r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="22"/>
+        <v>10</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>52</v>
+      </c>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row ht="45" r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="23"/>
+      <c r="E3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="37" t="s">
+        <v>52</v>
+      </c>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row ht="60" r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="24"/>
+        <v>15</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="38" t="s">
+        <v>52</v>
+      </c>
       <c r="G4" s="9"/>
     </row>
-    <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row ht="60" r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="39" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row ht="120" r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="25"/>
-    </row>
-    <row r="6" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="26"/>
+      <c r="E6" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="40" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C9" sqref="C8:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="17" collapsed="1"/>
-    <col min="2" max="2" width="33.140625" style="17" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25" style="17" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.140625" style="17" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.7109375" style="17" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="17" collapsed="1"/>
+    <col min="1" max="1" style="17" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="17" width="33.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="17" width="25.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="17" width="27.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="17" width="20.7109375" collapsed="true"/>
+    <col min="6" max="16384" style="17" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -943,110 +986,130 @@
         <v>4</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row ht="75" r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="18"/>
-      <c r="F2" s="27"/>
-    </row>
-    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="41" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row ht="90" r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="18"/>
-      <c r="F3" s="28"/>
-    </row>
-    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="42" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row ht="90" r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="18"/>
-      <c r="F4" s="29"/>
-    </row>
-    <row r="5" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="43" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row ht="135" r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="30"/>
-    </row>
-    <row r="6" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="44" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row ht="120" r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="18"/>
-      <c r="F6" s="31"/>
+        <v>31</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="45" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="35" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="36.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="34.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="22" width="12.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="36.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1066,58 +1129,70 @@
         <v>4</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row ht="90" r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="32"/>
-    </row>
-    <row r="3" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="46" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row ht="105" r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="33"/>
-    </row>
-    <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="47" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row ht="90" r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="34"/>
+        <v>37</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="48" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Improving SQL queries in test cases of Lesson 4
</commit_message>
<xml_diff>
--- a/AndyTEST/Libs/UserStoriesChecklist_02.xlsx
+++ b/AndyTEST/Libs/UserStoriesChecklist_02.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowHeight="8010" windowWidth="14805" xWindow="240" yWindow="105"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Story 1" r:id="rId1" sheetId="1"/>
-    <sheet name="Story 2" r:id="rId2" sheetId="2"/>
-    <sheet name="Story 3" r:id="rId3" sheetId="3"/>
+    <sheet name="Story 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Story 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Story 3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
   <si>
     <t>Test Case №</t>
   </si>
@@ -169,23 +169,13 @@
   </si>
   <si>
     <t>USE TestDB SELECT airline FROM Airlines INNER JOIN Flights ON Airlines.flightNumber = Flights.flightNumber GROUP BY airline HAVING AVG(averageTicketPrice) &lt; 100</t>
-  </si>
-  <si>
-    <t>1001;Munich;1002;New York;1003;Ottava;1004;Milan;1011;London;1012;Kiev;1013;Vilnius;1019;Ottava;1020;Vilnius;1021;Helsinki;1022;New York;1023;New York;1024;Milan;1025;London;1029;Kiev;1030;Helsinki;1031;Ottava;1033;Beijing;1034;Sydney;1035;Munich;</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>Fail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,6 +214,31 @@
     </font>
     <font>
       <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color indexed="10"/>
       <name val="Calibri"/>
     </font>
@@ -241,96 +256,6 @@
       <sz val="11"/>
       <color indexed="17"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="10"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="10"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="17"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="17"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="17"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="10"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
     </font>
   </fonts>
   <fills count="9">
@@ -404,108 +329,95 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="1" numFmtId="49" xfId="0">
+  <cellXfs count="36">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="3" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="4" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="5" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="6" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="7" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="8" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="23" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="24" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="26" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Обычный" xfId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -522,10 +434,10 @@
   <a:themeElements>
     <a:clrScheme name="Стандартная">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -560,7 +472,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -595,7 +507,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -683,7 +595,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -692,13 +604,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -708,7 +620,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -717,7 +629,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -726,7 +638,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -736,12 +648,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -772,7 +684,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -791,7 +703,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -803,22 +715,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="10" width="13.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="10" width="33.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="10" width="36.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="10" width="22.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="10" width="16.85546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="10" width="18.140625" collapsed="true"/>
-    <col min="7" max="16384" style="10" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="13.25" style="10" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.375" style="10" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="36.375" style="10" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.375" style="10" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.875" style="10" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.125" style="10" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.125" style="10" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -842,7 +754,7 @@
       </c>
       <c r="G1" s="9"/>
     </row>
-    <row ht="45" r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -855,15 +767,11 @@
       <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="36" t="s">
-        <v>52</v>
-      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="23"/>
       <c r="G2" s="9"/>
     </row>
-    <row ht="45" r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -876,15 +784,11 @@
       <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="37" t="s">
-        <v>52</v>
-      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="24"/>
       <c r="G3" s="9"/>
     </row>
-    <row ht="60" r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -897,15 +801,11 @@
       <c r="D4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="38" t="s">
-        <v>52</v>
-      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="25"/>
       <c r="G4" s="9"/>
     </row>
-    <row ht="60" r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
@@ -918,14 +818,10 @@
       <c r="D5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="39" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row ht="120" r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E5" s="11"/>
+      <c r="F5" s="26"/>
+    </row>
+    <row r="6" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>9</v>
       </c>
@@ -938,178 +834,154 @@
       <c r="D6" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="40" t="s">
-        <v>52</v>
-      </c>
+      <c r="E6" s="11"/>
+      <c r="F6" s="27"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C8:C9"/>
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.125" style="17" collapsed="1"/>
+    <col min="2" max="2" width="33.125" style="17" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25" style="17" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="27.125" style="17" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.75" style="17" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.125" style="17" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="18"/>
+      <c r="F2" s="28"/>
+    </row>
+    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="18"/>
+      <c r="F3" s="29"/>
+    </row>
+    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="18"/>
+      <c r="F4" s="30"/>
+    </row>
+    <row r="5" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="18"/>
+      <c r="F5" s="31"/>
+    </row>
+    <row r="6" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="18"/>
+      <c r="F6" s="32"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="17" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="17" width="33.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="17" width="25.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="17" width="27.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="17" width="20.7109375" collapsed="true"/>
-    <col min="6" max="16384" style="17" width="9.140625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row ht="30" r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row ht="75" r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="41" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row ht="90" r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="42" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row ht="90" r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="43" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row ht="135" r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="44" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row ht="120" r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="F6" s="45" t="s">
-        <v>53</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" customWidth="true" style="22" width="12.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="36.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="34.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="21.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="1" max="1" width="12.25" style="22" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="36.875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="34.125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1132,7 +1004,7 @@
         <v>21</v>
       </c>
     </row>
-    <row ht="90" r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -1145,14 +1017,10 @@
       <c r="D2" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="46" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row ht="105" r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E2" s="8"/>
+      <c r="F2" s="33"/>
+    </row>
+    <row r="3" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
@@ -1165,14 +1033,10 @@
       <c r="D3" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="47" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row ht="90" r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E3" s="8"/>
+      <c r="F3" s="34"/>
+    </row>
+    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
@@ -1185,14 +1049,10 @@
       <c r="D4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="48" t="s">
-        <v>52</v>
-      </c>
+      <c r="E4" s="8"/>
+      <c r="F4" s="35"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>